<commit_message>
fix #4, removed excessive DLY in excel
</commit_message>
<xml_diff>
--- a/MCP3561_SCAN_ModeSamplerate_Calculator.xlsx
+++ b/MCP3561_SCAN_ModeSamplerate_Calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\STM32\cubeide\f373cc_psd_mirror_control\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\mcp3564\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6259C8D5-A538-4F74-B969-63B45C1DE725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74AC1B4-25CA-4F66-9BCF-0A85BF90E439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="570" windowWidth="21600" windowHeight="10740" xr2:uid="{494F504D-9748-4D5D-8F75-D3B6136D8C9A}"/>
+    <workbookView xWindow="870" yWindow="4740" windowWidth="27750" windowHeight="15765" xr2:uid="{494F504D-9748-4D5D-8F75-D3B6136D8C9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,6 +133,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="##0.000E+0"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -266,7 +269,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="48" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -286,6 +288,7 @@
     <xf numFmtId="48" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="48" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,55 +349,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>571501</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>323851</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>40091</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFAC2007-86DF-4668-BC34-4DABAC4762A3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6429376" y="314325"/>
-          <a:ext cx="7067550" cy="2583266"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
@@ -508,6 +462,61 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>129639</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32150C62-27A1-20ED-450C-6498ED8CF362}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8216900" y="295275"/>
+          <a:ext cx="6104989" cy="2257425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -812,13 +821,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75DC5B3-2DFD-4969-B8ED-6292D2990485}">
   <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z31" sqref="Z31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="10" customWidth="1"/>
+    <col min="1" max="1" width="12" style="9" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
@@ -827,7 +836,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="9"/>
+      <c r="A1" s="8"/>
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -852,7 +861,7 @@
       <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
+      <c r="A2" s="8"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -877,13 +886,13 @@
       <c r="W2" s="2"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="19">
         <v>4915000</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -892,7 +901,7 @@
       <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <f>1/C3</f>
         <v>2.0345879959308239E-7</v>
       </c>
@@ -917,13 +926,13 @@
       <c r="W3" s="2"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" s="2"/>
@@ -948,13 +957,13 @@
       <c r="W4" s="2"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <f>C3/C4</f>
         <v>4915000</v>
       </c>
@@ -964,7 +973,7 @@
       <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <f>1/C5</f>
         <v>2.0345879959308239E-7</v>
       </c>
@@ -989,13 +998,13 @@
       <c r="W5" s="2"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <f>C5/4</f>
         <v>1228750</v>
       </c>
@@ -1005,7 +1014,7 @@
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <f>1/C6</f>
         <v>8.1383519837232957E-7</v>
       </c>
@@ -1030,13 +1039,13 @@
       <c r="W6" s="2"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <f>C6/C10</f>
         <v>299.98779296875</v>
       </c>
@@ -1046,7 +1055,7 @@
       <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <f>1/C7</f>
         <v>3.3334689725330619E-3</v>
       </c>
@@ -1071,7 +1080,7 @@
       <c r="W7" s="2"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1096,13 +1105,13 @@
       <c r="W8" s="2"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="A9" s="8">
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>4</v>
       </c>
       <c r="D9" s="2"/>
@@ -1127,20 +1136,20 @@
       <c r="W9" s="2"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
+      <c r="A10" s="8">
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <v>4096</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="11">
         <f>3*C11+(C12-1)*C11</f>
         <v>5120</v>
       </c>
@@ -1165,11 +1174,11 @@
       <c r="W10" s="2"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <f>IF(C10&gt;512,512,C10)</f>
         <v>512</v>
       </c>
@@ -1177,7 +1186,7 @@
       <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="18">
         <f>F10*F6</f>
         <v>4.166836215666327E-3</v>
       </c>
@@ -1204,11 +1213,11 @@
       <c r="W11" s="2"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <f>IF(C10&gt;512,C10/512,1)</f>
         <v>8</v>
       </c>
@@ -1216,7 +1225,7 @@
       <c r="E12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="18">
         <f>1/F11</f>
         <v>239.99023437500003</v>
       </c>
@@ -1243,13 +1252,13 @@
       <c r="W12" s="2"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="A13" s="8">
         <v>5</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="13">
         <v>512</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1276,13 +1285,13 @@
       <c r="W13" s="2"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="8">
         <v>6</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="17">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -1291,7 +1300,7 @@
       <c r="E14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="7">
         <f>C13*F6</f>
         <v>4.1668362156663274E-4</v>
       </c>
@@ -1316,7 +1325,7 @@
       <c r="W14" s="2"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="3"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -1341,21 +1350,21 @@
       <c r="W15" s="2"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <f>F10*F6</f>
         <v>4.166836215666327E-3</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="16">
         <f>1/C16</f>
         <v>239.99023437500003</v>
       </c>
@@ -1380,11 +1389,11 @@
       <c r="W16" s="2"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="8"/>
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <f>(C16+F14)</f>
         <v>4.5835198372329595E-3</v>
       </c>
@@ -1412,18 +1421,18 @@
       <c r="W17" s="2"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="7">
-        <f>C9*C17</f>
-        <v>1.8334079348931838E-2</v>
+      <c r="C18" s="6">
+        <f>C9*C17-F14</f>
+        <v>1.7917395727365205E-2</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -1444,11 +1453,11 @@
       <c r="W18" s="2"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <f>1/(C14)</f>
         <v>1</v>
       </c>
@@ -1476,13 +1485,13 @@
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <f>C19-C18</f>
-        <v>0.98166592065106817</v>
+        <v>0.98208260427263483</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>7</v>
@@ -1508,13 +1517,13 @@
       <c r="W20" s="2"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="16">
+      <c r="C21" s="15">
         <f>C20/F6</f>
-        <v>1206222</v>
+        <v>1206734</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>5</v>
@@ -1540,7 +1549,7 @@
       <c r="W21" s="2"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="3"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1565,7 +1574,7 @@
       <c r="W22" s="2"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="8"/>
       <c r="B23" s="3"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1590,7 +1599,7 @@
       <c r="W23" s="2"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="8"/>
       <c r="B24" s="3"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1615,7 +1624,7 @@
       <c r="W24" s="2"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="8"/>
       <c r="B25" s="3"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1640,7 +1649,7 @@
       <c r="W25" s="2"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="8"/>
       <c r="B26" s="3"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1665,7 +1674,7 @@
       <c r="W26" s="2"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="8"/>
       <c r="B27" s="3"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1690,7 +1699,7 @@
       <c r="W27" s="2"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="A28" s="8"/>
       <c r="B28" s="3"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1715,7 +1724,7 @@
       <c r="W28" s="2"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="8"/>
       <c r="B29" s="3"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>

</xml_diff>